<commit_message>
Auto-committed on 2023/07/04 週二 17:15:42.51
</commit_message>
<xml_diff>
--- a/Program/Other/LM049_底稿_放款金控法第44條利害關係人放款餘額表_限額控管.xlsx
+++ b/Program/Other/LM049_底稿_放款金控法第44條利害關係人放款餘額表_限額控管.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD35CF6-E34D-4C71-8E34-0BCF7CC0B171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5439E34-B62E-441D-8330-1466B2DB8D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="108.04金控子公司表7-1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'108.04金控子公司表7-1'!$A$3:$A$15</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'108.04金控子公司表7-1'!$B$1:$P$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'108.04金控子公司表7-1'!$B$1:$N$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'108.04金控子公司表7-1'!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
   <si>
     <t xml:space="preserve">      機密等級：機密</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -59,19 +59,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>十足擔保</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>不優於同類授信對象</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>達1億元且經董事會決議</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>符合金控法第44條</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -344,41 +336,35 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -396,7 +382,7 @@
     <xf numFmtId="10" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -408,158 +394,113 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -586,9 +527,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -626,9 +567,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -661,26 +602,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -713,26 +637,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -909,462 +816,392 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="22.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="1.21875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="26.77734375" style="26" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" style="4" customWidth="1"/>
-    <col min="4" max="5" width="15.109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="27" customWidth="1"/>
-    <col min="7" max="7" width="17.88671875" style="28" customWidth="1"/>
-    <col min="8" max="8" width="13" style="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="5.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="5.6640625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" style="6" customWidth="1"/>
-    <col min="13" max="13" width="21.77734375" style="6" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" style="31" customWidth="1"/>
-    <col min="16" max="16" width="11.88671875" style="32" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="4.54296875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.81640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="40.08984375" style="4" customWidth="1"/>
+    <col min="4" max="5" width="15.08984375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="17.90625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="13" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.90625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="17.90625" style="6" customWidth="1"/>
+    <col min="11" max="11" width="21.81640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.36328125" style="27" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" style="28" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="28.2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" ht="27.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
-      <c r="B1" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="38" t="s">
+      <c r="B1" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="33" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="66" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="67">
+    <row r="2" spans="1:14" ht="27.5" x14ac:dyDescent="0.4">
+      <c r="B2" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="53"/>
+      <c r="G2" s="54">
         <v>0</v>
       </c>
-      <c r="H2" s="67"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="68" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="69"/>
-    </row>
-    <row r="3" spans="1:16" s="10" customFormat="1" ht="198" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="59" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="50"/>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" ht="58.5" x14ac:dyDescent="0.4">
+      <c r="A3" s="7"/>
+      <c r="B3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="D3" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="41" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="47" t="s">
+      <c r="K3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="45" t="s">
+      <c r="M3" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="40" t="s">
+      <c r="N3" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
+    </row>
+    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="16"/>
       <c r="L4" s="17"/>
       <c r="M4" s="18"/>
       <c r="N4" s="19"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="21"/>
-    </row>
-    <row r="5" spans="1:16" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
-      <c r="B5" s="21" t="s">
+    </row>
+    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A5" s="20"/>
+      <c r="B5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+    </row>
+    <row r="6" spans="1:14" ht="58.5" x14ac:dyDescent="0.4">
+      <c r="A6" s="9"/>
+      <c r="B6" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="51"/>
+      <c r="F6" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="24"/>
-      <c r="P5" s="24"/>
-    </row>
-    <row r="6" spans="1:16" ht="198" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="40" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="70"/>
-      <c r="F6" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="47" t="s">
+      <c r="K6" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="44" t="s">
+      <c r="L6" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="45" t="s">
+      <c r="M6" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="40" t="s">
+      <c r="N6" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="P6" s="47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
+    </row>
+    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A7" s="20"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="16"/>
       <c r="L7" s="17"/>
       <c r="M7" s="18"/>
       <c r="N7" s="19"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="21"/>
-    </row>
-    <row r="8" spans="1:16" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
-      <c r="B8" s="21" t="s">
+    </row>
+    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+    </row>
+    <row r="9" spans="1:14" ht="58.5" x14ac:dyDescent="0.4">
+      <c r="B9" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="51"/>
+      <c r="F9" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-    </row>
-    <row r="9" spans="1:16" ht="198" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
-      <c r="B9" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="70"/>
-      <c r="F9" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="47" t="s">
+      <c r="K9" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="L9" s="44" t="s">
+      <c r="L9" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="M9" s="45" t="s">
+      <c r="M9" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="40" t="s">
+      <c r="N9" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="O9" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="P9" s="47" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
+    </row>
+    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16"/>
       <c r="L10" s="17"/>
       <c r="M10" s="18"/>
       <c r="N10" s="19"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
-    </row>
-    <row r="11" spans="1:16" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
-      <c r="B11" s="21" t="s">
+    </row>
+    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B11" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+    </row>
+    <row r="12" spans="1:14" ht="58.5" x14ac:dyDescent="0.4">
+      <c r="B12" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="51"/>
+      <c r="F12" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-    </row>
-    <row r="12" spans="1:16" ht="198" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
-      <c r="B12" s="59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="40" t="s">
+      <c r="I12" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="M12" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="70" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="70"/>
-      <c r="F12" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="G12" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12" s="47" t="s">
-        <v>9</v>
-      </c>
-      <c r="L12" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="M12" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="N12" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="O12" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12" s="47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
+    </row>
+    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16"/>
       <c r="L13" s="17"/>
       <c r="M13" s="18"/>
       <c r="N13" s="19"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="21"/>
-    </row>
-    <row r="14" spans="1:16" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="58"/>
+    </row>
+    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.4">
+      <c r="A14" s="20"/>
+      <c r="B14" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A15" s="20"/>
+      <c r="B15" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:A15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="8">
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="D3:E3"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B1:N1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="D3:E3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>